<commit_message>
Adapted file structure, added file_utils and yml config file
</commit_message>
<xml_diff>
--- a/test1.xlsx
+++ b/test1.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Franck</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -504,7 +504,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Franck</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>KEvin</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -552,7 +552,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>arr</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -584,7 +584,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KEvin</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -600,7 +600,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Dick</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -616,7 +616,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -648,7 +648,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jean</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -664,7 +664,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>arr</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -712,7 +712,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Evris</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -728,7 +728,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Dick</t>
+          <t>None</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -760,7 +760,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Evris</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Jean</t>
         </is>
       </c>
       <c r="C22" t="n">

</xml_diff>